<commit_message>
Finalized autonomated cta station id to google maps place id mapping
</commit_message>
<xml_diff>
--- a/CTA train stpids.xlsx
+++ b/CTA train stpids.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/59b2effe41531a4b/Documents/GitHub/T.A.U.I-Train-And-Uber-Integration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{E43ACFFE-5765-4E74-9666-41142F6CE423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43477572-C2D0-475C-B714-95AE2AEC878A}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{E43ACFFE-5765-4E74-9666-41142F6CE423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D9150DA-C490-42D2-AF49-4ACE86F33ADE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23640" windowHeight="15720" xr2:uid="{CB6DC720-3401-409A-97AA-A36CB99B3A09}"/>
+    <workbookView xWindow="1800" yWindow="3090" windowWidth="21600" windowHeight="11295" xr2:uid="{CB6DC720-3401-409A-97AA-A36CB99B3A09}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -543,6 +543,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -844,14 +848,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C268771D-1A48-4C14-BF60-37F0B3DF9FAB}">
   <dimension ref="A1:B142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="91.28515625" customWidth="1"/>
-    <col min="2" max="2" width="107.140625" customWidth="1"/>
+    <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="45.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.25">
@@ -862,7 +865,7 @@
         <v>40830</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -870,7 +873,7 @@
         <v>41120</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -910,7 +913,7 @@
         <v>40130</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="54" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -958,7 +961,7 @@
         <v>40450</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="54" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -982,7 +985,7 @@
         <v>41440</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -998,7 +1001,7 @@
         <v>41200</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1006,7 +1009,7 @@
         <v>40660</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="54" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1014,7 +1017,7 @@
         <v>40290</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="108" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -1022,7 +1025,7 @@
         <v>40170</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -1030,7 +1033,7 @@
         <v>41060</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="54" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -1038,7 +1041,7 @@
         <v>40010</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -1046,7 +1049,7 @@
         <v>41260</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="144" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="36" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -1054,7 +1057,7 @@
         <v>41320</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -1062,7 +1065,7 @@
         <v>40060</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -1070,7 +1073,7 @@
         <v>40340</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -1078,7 +1081,7 @@
         <v>41380</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -1086,7 +1089,7 @@
         <v>40440</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -1094,7 +1097,7 @@
         <v>41360</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="144" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="36" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -1102,7 +1105,7 @@
         <v>40570</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="54" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
@@ -1110,7 +1113,7 @@
         <v>40780</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
@@ -1118,7 +1121,7 @@
         <v>40280</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -1126,7 +1129,7 @@
         <v>41250</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
@@ -1134,7 +1137,7 @@
         <v>41000</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
@@ -1142,7 +1145,7 @@
         <v>41690</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
@@ -1150,7 +1153,7 @@
         <v>41410</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
@@ -1158,7 +1161,7 @@
         <v>40710</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
@@ -1166,7 +1169,7 @@
         <v>41450</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
@@ -1174,7 +1177,7 @@
         <v>40420</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="144" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="36" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>38</v>
       </c>
@@ -1182,7 +1185,7 @@
         <v>40970</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>39</v>
       </c>
@@ -1190,7 +1193,7 @@
         <v>40480</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="54" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>40</v>
       </c>
@@ -1198,7 +1201,7 @@
         <v>40630</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>41</v>
       </c>
@@ -1206,7 +1209,7 @@
         <v>40380</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>42</v>
       </c>
@@ -1214,7 +1217,7 @@
         <v>40430</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>43</v>
       </c>
@@ -1222,7 +1225,7 @@
         <v>41160</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="54" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>44</v>
       </c>
@@ -1230,7 +1233,7 @@
         <v>41670</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>45</v>
       </c>
@@ -1238,7 +1241,7 @@
         <v>40230</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>46</v>
       </c>
@@ -1246,7 +1249,7 @@
         <v>40090</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>47</v>
       </c>
@@ -1254,7 +1257,7 @@
         <v>40210</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="144" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="36" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>48</v>
       </c>
@@ -1270,7 +1273,7 @@
         <v>40050</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>50</v>
       </c>
@@ -1278,7 +1281,7 @@
         <v>40690</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>51</v>
       </c>
@@ -1286,7 +1289,7 @@
         <v>40140</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>52</v>
       </c>
@@ -1294,7 +1297,7 @@
         <v>40530</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>53</v>
       </c>
@@ -1302,7 +1305,7 @@
         <v>40320</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="54" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>54</v>
       </c>
@@ -1310,7 +1313,7 @@
         <v>40720</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>55</v>
       </c>
@@ -1326,7 +1329,7 @@
         <v>40520</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>57</v>
       </c>
@@ -1334,7 +1337,7 @@
         <v>40870</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>58</v>
       </c>
@@ -1342,7 +1345,7 @@
         <v>41220</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>59</v>
       </c>
@@ -1350,7 +1353,7 @@
         <v>40510</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>60</v>
       </c>
@@ -1358,7 +1361,7 @@
         <v>41170</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="54" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>61</v>
       </c>
@@ -1366,7 +1369,7 @@
         <v>40490</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="54" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>62</v>
       </c>
@@ -1374,7 +1377,7 @@
         <v>40330</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>63</v>
       </c>
@@ -1382,7 +1385,7 @@
         <v>40760</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>64</v>
       </c>
@@ -1390,7 +1393,7 @@
         <v>40940</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>65</v>
       </c>
@@ -1398,7 +1401,7 @@
         <v>41130</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="144" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="36" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>66</v>
       </c>
@@ -1406,7 +1409,7 @@
         <v>40980</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>67</v>
       </c>
@@ -1414,7 +1417,7 @@
         <v>40020</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="144" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" ht="36" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>68</v>
       </c>
@@ -1422,7 +1425,7 @@
         <v>40750</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="144" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="36" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>69</v>
       </c>
@@ -1430,7 +1433,7 @@
         <v>40850</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>70</v>
       </c>
@@ -1438,7 +1441,7 @@
         <v>41490</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>71</v>
       </c>
@@ -1446,7 +1449,7 @@
         <v>40900</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>72</v>
       </c>
@@ -1454,7 +1457,7 @@
         <v>40810</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>73</v>
       </c>
@@ -1462,7 +1465,7 @@
         <v>40300</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>74</v>
       </c>
@@ -1470,7 +1473,7 @@
         <v>40550</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>75</v>
       </c>
@@ -1478,7 +1481,7 @@
         <v>41460</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>76</v>
       </c>
@@ -1486,7 +1489,7 @@
         <v>40070</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>77</v>
       </c>
@@ -1502,7 +1505,7 @@
         <v>41190</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="54" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>79</v>
       </c>
@@ -1510,7 +1513,7 @@
         <v>41280</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>80</v>
       </c>
@@ -1518,7 +1521,7 @@
         <v>41180</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>81</v>
       </c>
@@ -1526,7 +1529,7 @@
         <v>41040</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>82</v>
       </c>
@@ -1534,7 +1537,7 @@
         <v>41070</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="108" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>83</v>
       </c>
@@ -1542,7 +1545,7 @@
         <v>40250</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>84</v>
       </c>
@@ -1550,7 +1553,7 @@
         <v>41150</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>85</v>
       </c>
@@ -1558,7 +1561,7 @@
         <v>41290</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>86</v>
       </c>
@@ -1566,7 +1569,7 @@
         <v>41140</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>87</v>
       </c>
@@ -1582,7 +1585,7 @@
         <v>41660</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>89</v>
       </c>
@@ -1590,7 +1593,7 @@
         <v>40700</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>90</v>
       </c>
@@ -1598,7 +1601,7 @@
         <v>41340</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="54" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>91</v>
       </c>
@@ -1606,7 +1609,7 @@
         <v>40160</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>92</v>
       </c>
@@ -1614,7 +1617,7 @@
         <v>40770</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>93</v>
       </c>
@@ -1622,7 +1625,7 @@
         <v>41050</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="54" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>94</v>
       </c>
@@ -1630,7 +1633,7 @@
         <v>41020</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>95</v>
       </c>
@@ -1646,7 +1649,7 @@
         <v>40270</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>97</v>
       </c>
@@ -1654,7 +1657,7 @@
         <v>40930</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>98</v>
       </c>
@@ -1662,7 +1665,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>99</v>
       </c>
@@ -1670,7 +1673,7 @@
         <v>41090</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>100</v>
       </c>
@@ -1678,7 +1681,7 @@
         <v>41330</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>101</v>
       </c>
@@ -1686,7 +1689,7 @@
         <v>41500</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>102</v>
       </c>
@@ -1702,7 +1705,7 @@
         <v>40100</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="54" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>104</v>
       </c>
@@ -1718,7 +1721,7 @@
         <v>40400</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>106</v>
       </c>
@@ -1726,7 +1729,7 @@
         <v>40180</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>107</v>
       </c>
@@ -1734,7 +1737,7 @@
         <v>41350</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>108</v>
       </c>
@@ -1742,7 +1745,7 @@
         <v>41680</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>109</v>
       </c>
@@ -1750,7 +1753,7 @@
         <v>40890</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>110</v>
       </c>
@@ -1766,7 +1769,7 @@
         <v>41030</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>112</v>
       </c>
@@ -1774,7 +1777,7 @@
         <v>40150</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="144" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" ht="36" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>113</v>
       </c>
@@ -1782,7 +1785,7 @@
         <v>40920</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>114</v>
       </c>
@@ -1790,7 +1793,7 @@
         <v>40030</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>115</v>
       </c>
@@ -1798,7 +1801,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="54" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>116</v>
       </c>
@@ -1806,7 +1809,7 @@
         <v>40040</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>117</v>
       </c>
@@ -1814,7 +1817,7 @@
         <v>40470</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>118</v>
       </c>
@@ -1822,7 +1825,7 @@
         <v>40610</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>119</v>
       </c>
@@ -1830,7 +1833,7 @@
         <v>41010</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>120</v>
       </c>
@@ -1838,7 +1841,7 @@
         <v>41400</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>121</v>
       </c>
@@ -1846,7 +1849,7 @@
         <v>40820</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>122</v>
       </c>
@@ -1854,7 +1857,7 @@
         <v>40800</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>123</v>
       </c>
@@ -1862,7 +1865,7 @@
         <v>40080</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="54" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>124</v>
       </c>
@@ -1870,7 +1873,7 @@
         <v>40840</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>125</v>
       </c>
@@ -1878,7 +1881,7 @@
         <v>40360</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>126</v>
       </c>
@@ -1886,7 +1889,7 @@
         <v>40190</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>127</v>
       </c>
@@ -1894,7 +1897,7 @@
         <v>40260</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>128</v>
       </c>
@@ -1902,7 +1905,7 @@
         <v>40880</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="54" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>129</v>
       </c>
@@ -1910,7 +1913,7 @@
         <v>40350</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>130</v>
       </c>
@@ -1918,7 +1921,7 @@
         <v>41700</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="54" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>131</v>
       </c>
@@ -1926,7 +1929,7 @@
         <v>40730</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>132</v>
       </c>
@@ -1934,7 +1937,7 @@
         <v>40370</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>133</v>
       </c>
@@ -1942,7 +1945,7 @@
         <v>41210</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>134</v>
       </c>
@@ -1950,7 +1953,7 @@
         <v>41480</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="72" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>135</v>
       </c>
@@ -1958,7 +1961,7 @@
         <v>40740</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="144" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" ht="36" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>136</v>
       </c>
@@ -1966,7 +1969,7 @@
         <v>40220</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="144" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" ht="36" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>137</v>
       </c>
@@ -1974,7 +1977,7 @@
         <v>40670</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>138</v>
       </c>
@@ -1982,7 +1985,7 @@
         <v>40310</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>139</v>
       </c>
@@ -1992,5 +1995,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
able to get all trains and times
</commit_message>
<xml_diff>
--- a/CTA train stpids.xlsx
+++ b/CTA train stpids.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="17" documentId="8_{E43ACFFE-5765-4E74-9666-41142F6CE423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D9150DA-C490-42D2-AF49-4ACE86F33ADE}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="3090" windowWidth="21600" windowHeight="11295" xr2:uid="{CB6DC720-3401-409A-97AA-A36CB99B3A09}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CB6DC720-3401-409A-97AA-A36CB99B3A09}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -848,7 +848,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C268771D-1A48-4C14-BF60-37F0B3DF9FAB}">
   <dimension ref="A1:B142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>